<commit_message>
added folder reader program
</commit_message>
<xml_diff>
--- a/t_Batch1.xlsx
+++ b/t_Batch1.xlsx
@@ -8,14 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://morningstaronline-my.sharepoint.com/personal/spencer_klug_pitchbook_com/Documents/India_PF_Expansion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_7A59A643827310DEEC4C5CD4475DCE3A874B7A6E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EFD8C845-293C-4A41-A945-ADD13867EA01}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="11_7A59A643827310DEEC4C5CD4475DCE3A874B7A6E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{40161A58-D946-4808-9F19-C5467A10B8FA}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="4290" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AP$501</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -2863,7 +2877,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -2877,6 +2891,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2920,7 +2935,7 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3223,15 +3238,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AP501"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.7109375" customWidth="1"/>
+    <col min="3" max="3" width="246.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
@@ -3401,7 +3420,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2500</v>
       </c>
@@ -3418,7 +3437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2501</v>
       </c>
@@ -3435,7 +3454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2502</v>
       </c>
@@ -3534,7 +3553,7 @@
         <v>57719929</v>
       </c>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2505</v>
       </c>
@@ -3551,7 +3570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2506</v>
       </c>
@@ -3568,7 +3587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2507</v>
       </c>
@@ -3585,7 +3604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2508</v>
       </c>
@@ -3602,7 +3621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2509</v>
       </c>
@@ -3719,7 +3738,7 @@
         <v>3365672480</v>
       </c>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2512</v>
       </c>
@@ -3777,7 +3796,7 @@
         <v>700000</v>
       </c>
     </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2514</v>
       </c>
@@ -4178,7 +4197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2518</v>
       </c>
@@ -4195,7 +4214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2519</v>
       </c>
@@ -4212,7 +4231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2520</v>
       </c>
@@ -4229,7 +4248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2521</v>
       </c>
@@ -4408,7 +4427,7 @@
         <v>88763308</v>
       </c>
     </row>
-    <row r="27" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2525</v>
       </c>
@@ -4425,7 +4444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2526</v>
       </c>
@@ -4442,7 +4461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2527</v>
       </c>
@@ -4459,7 +4478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2528</v>
       </c>
@@ -4517,7 +4536,7 @@
         <v>40402</v>
       </c>
     </row>
-    <row r="32" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2530</v>
       </c>
@@ -4575,7 +4594,7 @@
         <v>-49399460</v>
       </c>
     </row>
-    <row r="34" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2532</v>
       </c>
@@ -4592,7 +4611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2533</v>
       </c>
@@ -4609,7 +4628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2534</v>
       </c>
@@ -4626,7 +4645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2535</v>
       </c>
@@ -4643,7 +4662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2536</v>
       </c>
@@ -4660,7 +4679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2537</v>
       </c>
@@ -4789,7 +4808,7 @@
         <v>109312685</v>
       </c>
     </row>
-    <row r="42" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2540</v>
       </c>
@@ -6141,7 +6160,7 @@
         <v>-202</v>
       </c>
     </row>
-    <row r="58" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2556</v>
       </c>
@@ -6158,7 +6177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2557</v>
       </c>
@@ -6175,7 +6194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2558</v>
       </c>
@@ -6698,7 +6717,7 @@
         <v>2957259</v>
       </c>
     </row>
-    <row r="65" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>2563</v>
       </c>
@@ -7259,7 +7278,7 @@
         <v>1887472</v>
       </c>
     </row>
-    <row r="74" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>2572</v>
       </c>
@@ -7792,7 +7811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>2579</v>
       </c>
@@ -7809,7 +7828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>2580</v>
       </c>
@@ -8335,7 +8354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>2585</v>
       </c>
@@ -8352,7 +8371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>2586</v>
       </c>
@@ -8369,7 +8388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>2587</v>
       </c>
@@ -9701,7 +9720,7 @@
         <v>21151</v>
       </c>
     </row>
-    <row r="101" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>2599</v>
       </c>
@@ -9718,7 +9737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>2600</v>
       </c>
@@ -9735,7 +9754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>2601</v>
       </c>
@@ -9752,7 +9771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>2602</v>
       </c>
@@ -9769,7 +9788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>2603</v>
       </c>
@@ -9786,7 +9805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>2604</v>
       </c>
@@ -9803,7 +9822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>2605</v>
       </c>
@@ -9974,7 +9993,7 @@
         <v>23177551</v>
       </c>
     </row>
-    <row r="110" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>2608</v>
       </c>
@@ -10620,7 +10639,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="118" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>2616</v>
       </c>
@@ -10637,7 +10656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>2617</v>
       </c>
@@ -10654,7 +10673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>2618</v>
       </c>
@@ -11881,7 +11900,7 @@
         <v>114572</v>
       </c>
     </row>
-    <row r="138" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>2636</v>
       </c>
@@ -11898,7 +11917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>2637</v>
       </c>
@@ -11915,7 +11934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>2638</v>
       </c>
@@ -11932,7 +11951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>2639</v>
       </c>
@@ -11949,7 +11968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>2640</v>
       </c>
@@ -12535,7 +12554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>2648</v>
       </c>
@@ -12552,7 +12571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>2649</v>
       </c>
@@ -12569,7 +12588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>2650</v>
       </c>
@@ -12586,7 +12605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>2651</v>
       </c>
@@ -12826,7 +12845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>2654</v>
       </c>
@@ -12843,7 +12862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>2655</v>
       </c>
@@ -12860,7 +12879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>2656</v>
       </c>
@@ -12877,7 +12896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>2657</v>
       </c>
@@ -12894,7 +12913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>2658</v>
       </c>
@@ -13117,7 +13136,7 @@
         <v>3682587</v>
       </c>
     </row>
-    <row r="165" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>2663</v>
       </c>
@@ -13134,7 +13153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>2664</v>
       </c>
@@ -13151,7 +13170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>2665</v>
       </c>
@@ -13168,7 +13187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>2666</v>
       </c>
@@ -13349,7 +13368,7 @@
         <v>2900</v>
       </c>
     </row>
-    <row r="173" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>2671</v>
       </c>
@@ -13366,7 +13385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>2672</v>
       </c>
@@ -13383,7 +13402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>2673</v>
       </c>
@@ -13400,7 +13419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>2674</v>
       </c>
@@ -13417,7 +13436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>2675</v>
       </c>
@@ -13434,7 +13453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>2676</v>
       </c>
@@ -13451,7 +13470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>2677</v>
       </c>
@@ -13571,7 +13590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>2680</v>
       </c>
@@ -13588,7 +13607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>2681</v>
       </c>
@@ -15614,7 +15633,7 @@
         <v>10908968</v>
       </c>
     </row>
-    <row r="206" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>2704</v>
       </c>
@@ -15631,7 +15650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>2705</v>
       </c>
@@ -15648,7 +15667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>2706</v>
       </c>
@@ -15665,7 +15684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>2707</v>
       </c>
@@ -15682,7 +15701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>2708</v>
       </c>
@@ -15699,7 +15718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>2709</v>
       </c>
@@ -15716,7 +15735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>2710</v>
       </c>
@@ -15733,7 +15752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>2711</v>
       </c>
@@ -15750,7 +15769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>2712</v>
       </c>
@@ -15767,7 +15786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>2713</v>
       </c>
@@ -15872,7 +15891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>2716</v>
       </c>
@@ -15889,7 +15908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>2717</v>
       </c>
@@ -15906,7 +15925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>2718</v>
       </c>
@@ -15923,7 +15942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>2719</v>
       </c>
@@ -17149,7 +17168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>2732</v>
       </c>
@@ -17166,7 +17185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>2733</v>
       </c>
@@ -17183,7 +17202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>2734</v>
       </c>
@@ -17200,7 +17219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>2735</v>
       </c>
@@ -17273,7 +17292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>2737</v>
       </c>
@@ -17290,7 +17309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>2738</v>
       </c>
@@ -17307,7 +17326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>2739</v>
       </c>
@@ -17324,7 +17343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>2740</v>
       </c>
@@ -17382,7 +17401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>2742</v>
       </c>
@@ -17399,7 +17418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>2743</v>
       </c>
@@ -17416,7 +17435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>2744</v>
       </c>
@@ -17433,7 +17452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>2745</v>
       </c>
@@ -17450,7 +17469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>2746</v>
       </c>
@@ -17467,7 +17486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>2747</v>
       </c>
@@ -17484,7 +17503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>2748</v>
       </c>
@@ -17613,7 +17632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>2751</v>
       </c>
@@ -17712,7 +17731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>2754</v>
       </c>
@@ -17729,7 +17748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>2755</v>
       </c>
@@ -17746,7 +17765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258">
         <v>2756</v>
       </c>
@@ -17763,7 +17782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259">
         <v>2757</v>
       </c>
@@ -18357,7 +18376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>2763</v>
       </c>
@@ -18374,7 +18393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266">
         <v>2764</v>
       </c>
@@ -18391,7 +18410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267">
         <v>2765</v>
       </c>
@@ -18408,7 +18427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268">
         <v>2766</v>
       </c>
@@ -18425,7 +18444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269">
         <v>2767</v>
       </c>
@@ -18442,7 +18461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270">
         <v>2768</v>
       </c>
@@ -18459,7 +18478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271">
         <v>2769</v>
       </c>
@@ -18857,7 +18876,7 @@
         <v>-58962742</v>
       </c>
     </row>
-    <row r="278" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278">
         <v>2776</v>
       </c>
@@ -18874,7 +18893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279">
         <v>2777</v>
       </c>
@@ -18891,7 +18910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280">
         <v>2778</v>
       </c>
@@ -18908,7 +18927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="281" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281">
         <v>2779</v>
       </c>
@@ -18925,7 +18944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282">
         <v>2780</v>
       </c>
@@ -18942,7 +18961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>2781</v>
       </c>
@@ -18959,7 +18978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>2782</v>
       </c>
@@ -19180,7 +19199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288">
         <v>2786</v>
       </c>
@@ -20287,7 +20306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>2798</v>
       </c>
@@ -20304,7 +20323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>2799</v>
       </c>
@@ -20321,7 +20340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="302" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A302">
         <v>2800</v>
       </c>
@@ -21828,7 +21847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="319" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A319">
         <v>2817</v>
       </c>
@@ -21845,7 +21864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="320" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A320">
         <v>2818</v>
       </c>
@@ -21862,7 +21881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="321" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A321">
         <v>2819</v>
       </c>
@@ -21879,7 +21898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="322" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A322">
         <v>2820</v>
       </c>
@@ -22269,7 +22288,7 @@
         <v>1324</v>
       </c>
     </row>
-    <row r="331" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A331">
         <v>2829</v>
       </c>
@@ -22286,7 +22305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="332" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A332">
         <v>2830</v>
       </c>
@@ -22303,7 +22322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="333" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A333">
         <v>2831</v>
       </c>
@@ -22320,7 +22339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="334" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A334">
         <v>2832</v>
       </c>
@@ -22337,7 +22356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="335" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A335">
         <v>2833</v>
       </c>
@@ -22354,7 +22373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="336" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A336">
         <v>2834</v>
       </c>
@@ -22539,7 +22558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="340" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A340">
         <v>2838</v>
       </c>
@@ -22597,7 +22616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="342" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A342">
         <v>2840</v>
       </c>
@@ -22614,7 +22633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="343" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A343">
         <v>2841</v>
       </c>
@@ -22631,7 +22650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="344" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A344">
         <v>2842</v>
       </c>
@@ -25458,7 +25477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="376" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A376">
         <v>2874</v>
       </c>
@@ -25475,7 +25494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="377" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A377">
         <v>2875</v>
       </c>
@@ -25492,7 +25511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="378" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A378">
         <v>2876</v>
       </c>
@@ -25509,7 +25528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="379" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A379">
         <v>2877</v>
       </c>
@@ -25688,7 +25707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="383" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A383">
         <v>2881</v>
       </c>
@@ -25705,7 +25724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="384" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A384">
         <v>2882</v>
       </c>
@@ -25722,7 +25741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="385" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A385">
         <v>2883</v>
       </c>
@@ -25739,7 +25758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="386" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A386">
         <v>2884</v>
       </c>
@@ -25859,7 +25878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="389" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A389">
         <v>2887</v>
       </c>
@@ -25876,7 +25895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="390" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A390">
         <v>2888</v>
       </c>
@@ -25893,7 +25912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="391" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A391">
         <v>2889</v>
       </c>
@@ -25910,7 +25929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="392" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A392">
         <v>2890</v>
       </c>
@@ -26888,7 +26907,7 @@
         <v>254054</v>
       </c>
     </row>
-    <row r="401" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A401">
         <v>2899</v>
       </c>
@@ -26905,7 +26924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="402" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A402">
         <v>2900</v>
       </c>
@@ -26922,7 +26941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="403" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A403">
         <v>2901</v>
       </c>
@@ -27762,7 +27781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="412" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A412">
         <v>2910</v>
       </c>
@@ -27779,7 +27798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="413" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A413">
         <v>2911</v>
       </c>
@@ -27796,7 +27815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="414" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A414">
         <v>2912</v>
       </c>
@@ -29062,7 +29081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="429" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A429">
         <v>2927</v>
       </c>
@@ -29079,7 +29098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="430" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A430">
         <v>2928</v>
       </c>
@@ -29096,7 +29115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="431" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A431">
         <v>2929</v>
       </c>
@@ -29113,7 +29132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="432" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A432">
         <v>2930</v>
       </c>
@@ -29130,7 +29149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="433" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A433">
         <v>2931</v>
       </c>
@@ -29147,7 +29166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="434" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A434">
         <v>2932</v>
       </c>
@@ -29164,7 +29183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="435" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A435">
         <v>2933</v>
       </c>
@@ -29181,7 +29200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="436" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A436">
         <v>2934</v>
       </c>
@@ -32075,7 +32094,7 @@
         <v>-14950</v>
       </c>
     </row>
-    <row r="473" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A473">
         <v>2971</v>
       </c>
@@ -33372,7 +33391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="484" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A484">
         <v>2982</v>
       </c>
@@ -33389,7 +33408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="485" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="485" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A485">
         <v>2983</v>
       </c>
@@ -33406,7 +33425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="486" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A486">
         <v>2984</v>
       </c>
@@ -33535,7 +33554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="489" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="489" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A489">
         <v>2987</v>
       </c>
@@ -33552,7 +33571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="490" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="490" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A490">
         <v>2988</v>
       </c>
@@ -33569,7 +33588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="491" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="491" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A491">
         <v>2989</v>
       </c>
@@ -33668,7 +33687,7 @@
         <v>2499</v>
       </c>
     </row>
-    <row r="494" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="494" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A494">
         <v>2992</v>
       </c>
@@ -33685,7 +33704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="495" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="495" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A495">
         <v>2993</v>
       </c>
@@ -33702,7 +33721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="496" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="496" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A496">
         <v>2994</v>
       </c>
@@ -33719,7 +33738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="497" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="497" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A497">
         <v>2995</v>
       </c>
@@ -33736,7 +33755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="498" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="498" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A498">
         <v>2996</v>
       </c>
@@ -33753,7 +33772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="499" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="499" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A499">
         <v>2997</v>
       </c>
@@ -33883,6 +33902,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AP501" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="5">
+      <filters>
+        <filter val="TRUE"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>